<commit_message>
adding input files for ensemble
</commit_message>
<xml_diff>
--- a/journalnew.xlsx
+++ b/journalnew.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t xml:space="preserve">NEURAL NET TUNING</t>
   </si>
@@ -119,6 +119,42 @@
   </si>
   <si>
     <t xml:space="preserve">learning rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSEMBLE LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preds file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fasttext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lgbm_olivier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capsulenet_eric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stacknet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logreg_bojan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb_svm dimitryov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanketeking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">blend of blends</t>
   </si>
 </sst>
 </file>
@@ -303,16 +339,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:N18"/>
+  <dimension ref="C2:N34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
@@ -541,6 +577,86 @@
       </c>
       <c r="E18" s="0" t="n">
         <v>0.9764</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.98856</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.9852</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.9764</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0.984</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0.9779</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>